<commit_message>
Updating Framework Files AK
</commit_message>
<xml_diff>
--- a/src/main/java/Resources/ReadData.xlsx
+++ b/src/main/java/Resources/ReadData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>FirstRow</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Abhi2</t>
+  </si>
+  <si>
+    <t>Abhi_0</t>
+  </si>
+  <si>
+    <t>Abhi_1</t>
+  </si>
+  <si>
+    <t>Abhi_2</t>
   </si>
 </sst>
 </file>
@@ -407,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -475,6 +484,72 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding Log4j changes : AK
</commit_message>
<xml_diff>
--- a/src/main/java/Resources/ReadData.xlsx
+++ b/src/main/java/Resources/ReadData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
   <si>
     <t>FirstRow</t>
   </si>
@@ -416,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -547,6 +547,72 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Extent Reports, Log4J changes : AK
</commit_message>
<xml_diff>
--- a/src/main/java/Resources/ReadData.xlsx
+++ b/src/main/java/Resources/ReadData.xlsx
@@ -16,42 +16,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>FirstRow</t>
   </si>
   <si>
-    <t>FirstCell</t>
-  </si>
-  <si>
     <t>SecondRow</t>
   </si>
   <si>
     <t>ThirdRow</t>
   </si>
   <si>
-    <t>abhishek</t>
-  </si>
-  <si>
-    <t>Abhi0</t>
-  </si>
-  <si>
-    <t>Abhi1</t>
-  </si>
-  <si>
     <t>SecondCell</t>
   </si>
   <si>
-    <t>FirstCell_1</t>
-  </si>
-  <si>
     <t>SecondCell_2</t>
   </si>
   <si>
-    <t>Abhishek_1</t>
-  </si>
-  <si>
-    <t>Abhi2</t>
+    <t>Khatod</t>
+  </si>
+  <si>
+    <t>RowName</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>SecondCell_1</t>
+  </si>
+  <si>
+    <t>ThirdCell_1</t>
+  </si>
+  <si>
+    <t>ThirdCell</t>
+  </si>
+  <si>
+    <t>ThirdCell_2</t>
   </si>
   <si>
     <t>Abhi_0</t>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -429,191 +432,84 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>